<commit_message>
Added empty sheet to the test file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2018" sheetId="3" r:id="rId1"/>
     <sheet name="2017" sheetId="1" r:id="rId2"/>
-    <sheet name="2016" sheetId="2" r:id="rId3"/>
+    <sheet name="No Data" sheetId="5" r:id="rId3"/>
+    <sheet name="2016" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -404,7 +405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -628,6 +629,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>